<commit_message>
updated meeting minutes 2
</commit_message>
<xml_diff>
--- a/RequestITMeetings.xlsx
+++ b/RequestITMeetings.xlsx
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -547,6 +547,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>